<commit_message>
Added/fixed some more stuff
</commit_message>
<xml_diff>
--- a/input_file.xlsx
+++ b/input_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mxs1113\PycharmProjects\Markosim Re-Build v1.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mxs1113\PycharmProjects\markosim_reloaded\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -87,8 +87,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,21 +396,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
     <col min="6" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="8" width="7.5703125" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" customWidth="1"/>
     <col min="10" max="10" width="5.7109375" customWidth="1"/>
@@ -449,8 +450,9 @@
       <c r="B2">
         <v>600</v>
       </c>
-      <c r="C2">
-        <v>300</v>
+      <c r="C2" s="1">
+        <f>200*SQRT(2)</f>
+        <v>282.84271247461902</v>
       </c>
       <c r="D2">
         <v>0.8</v>
@@ -461,25 +463,26 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>60</v>
       </c>
       <c r="H2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>100</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>600</v>
       </c>
-      <c r="C3">
-        <v>300</v>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C13" si="0">200*SQRT(2)</f>
+        <v>282.84271247461902</v>
       </c>
       <c r="D3">
         <v>0.8</v>
@@ -488,20 +491,584 @@
         <v>1</v>
       </c>
       <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>600</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D4">
+        <v>0.8</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4" s="1">
+        <v>60</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>600</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D5">
+        <v>0.8</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1">
+        <v>60</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>600</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D6">
+        <v>-0.8</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>5</v>
       </c>
-      <c r="G3">
-        <v>60</v>
-      </c>
-      <c r="H3">
+      <c r="G6" s="1">
+        <v>60</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>600</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D7">
+        <v>-0.8</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1">
+        <v>60</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>600</v>
+      </c>
+      <c r="C8" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D8">
+        <v>-0.8</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>15</v>
+      </c>
+      <c r="G8" s="1">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>600</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D9">
+        <v>-0.8</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1">
+        <v>60</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>600</v>
+      </c>
+      <c r="C10" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>5</v>
       </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
+      <c r="G10" s="1">
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>600</v>
+      </c>
+      <c r="C11" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" s="1">
+        <v>60</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>600</v>
+      </c>
+      <c r="C12" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1">
+        <v>60</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>600</v>
+      </c>
+      <c r="C13" s="1">
+        <f t="shared" si="0"/>
+        <v>282.84271247461902</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1">
+        <v>60</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="1"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="1"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="1"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="1"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="1"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="1"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="1"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="1"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="1"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="1"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="1"/>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="1"/>
+      <c r="G49" s="1"/>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="1"/>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="1"/>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="1"/>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="1"/>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="1"/>
+      <c r="G55" s="1"/>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="1"/>
+      <c r="G56" s="1"/>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C57" s="1"/>
+      <c r="G57" s="1"/>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C58" s="1"/>
+      <c r="G58" s="1"/>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="1"/>
+      <c r="G59" s="1"/>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C60" s="1"/>
+      <c r="G60" s="1"/>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C61" s="1"/>
+      <c r="G61" s="1"/>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="1"/>
+      <c r="G62" s="1"/>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C63" s="1"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C64" s="1"/>
+      <c r="G64" s="1"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65" s="1"/>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C66" s="1"/>
+      <c r="G66" s="1"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C67" s="1"/>
+      <c r="G67" s="1"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+      <c r="G68" s="1"/>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C69" s="1"/>
+      <c r="G69" s="1"/>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C70" s="1"/>
+      <c r="G70" s="1"/>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C71" s="1"/>
+      <c r="G71" s="1"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C72" s="1"/>
+      <c r="G72" s="1"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C73" s="1"/>
+      <c r="G73" s="1"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C74" s="1"/>
+      <c r="G74" s="1"/>
+    </row>
+    <row r="75" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C75" s="1"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C76" s="1"/>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C77" s="1"/>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C78" s="1"/>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C79" s="1"/>
+      <c r="G79" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1">

</xml_diff>